<commit_message>
updated implementation results file
</commit_message>
<xml_diff>
--- a/Thesis_Implementation_results.xlsx
+++ b/Thesis_Implementation_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gauravshetty/Documents/InSoSySc/4th Sem/Thesis/Mobi Thesis /Thesis_Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD5888D-7403-7149-B5F1-39CC625073FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9181E4-E4CE-D049-90A2-12766016F007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32400" yWindow="4160" windowWidth="30520" windowHeight="21320" xr2:uid="{C18249C4-D491-7445-A020-EC05014236CF}"/>
+    <workbookView xWindow="26100" yWindow="4820" windowWidth="36420" windowHeight="20540" xr2:uid="{C18249C4-D491-7445-A020-EC05014236CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Controlled Low Rate</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Projection First, Then Selection Bid stream</t>
+  </si>
+  <si>
+    <t>All latency values are in milliseconds (ms)</t>
   </si>
 </sst>
 </file>
@@ -204,10 +207,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B78CE49-B45A-6E44-BF80-5AC389AFBAEA}">
-  <dimension ref="A1:AL5"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,587 +596,632 @@
     <col min="38" max="38" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="1" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+    </row>
+    <row r="2" spans="1:38" s="1" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:38" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>49999</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>10004</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>249967</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>10003</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>10005</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>50004</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>50003</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>10004</v>
       </c>
-      <c r="J2">
+      <c r="J3">
         <v>50000</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <v>50004</v>
       </c>
-      <c r="L2">
+      <c r="L3">
         <v>50003</v>
       </c>
-      <c r="M2">
+      <c r="M3">
         <v>10006</v>
       </c>
-      <c r="N2">
+      <c r="N3">
         <v>10013</v>
       </c>
-      <c r="O2">
+      <c r="O3">
+        <v>50004</v>
+      </c>
+      <c r="P3">
+        <v>10006</v>
+      </c>
+      <c r="Q3">
         <v>50009</v>
       </c>
-      <c r="P2">
+      <c r="R3">
+        <v>10004</v>
+      </c>
+      <c r="S3">
+        <v>50006</v>
+      </c>
+      <c r="T3">
+        <v>10007</v>
+      </c>
+      <c r="U3">
+        <v>50006</v>
+      </c>
+      <c r="V3">
         <v>10005</v>
       </c>
-      <c r="Q2">
-        <v>50009</v>
-      </c>
-      <c r="R2">
-        <v>10004</v>
-      </c>
-      <c r="S2">
+      <c r="W3">
+        <v>50005</v>
+      </c>
+      <c r="X3">
+        <v>10005</v>
+      </c>
+      <c r="Y3">
+        <v>50001</v>
+      </c>
+      <c r="Z3">
+        <v>10005</v>
+      </c>
+      <c r="AA3">
+        <v>50005</v>
+      </c>
+      <c r="AB3">
+        <v>10011</v>
+      </c>
+      <c r="AC3">
+        <v>10545</v>
+      </c>
+      <c r="AD3">
+        <v>50071</v>
+      </c>
+      <c r="AE3">
+        <v>10932</v>
+      </c>
+      <c r="AF3">
+        <v>50001</v>
+      </c>
+      <c r="AG3">
+        <v>11322</v>
+      </c>
+      <c r="AH3">
+        <v>50010</v>
+      </c>
+      <c r="AI3">
+        <v>11941</v>
+      </c>
+      <c r="AJ3">
+        <v>249998</v>
+      </c>
+      <c r="AK3">
+        <v>12053</v>
+      </c>
+      <c r="AL3">
+        <v>250018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>249998</v>
+      </c>
+      <c r="C4">
         <v>50006</v>
       </c>
-      <c r="T2">
-        <v>10007</v>
-      </c>
-      <c r="U2">
-        <v>50006</v>
-      </c>
-      <c r="V2">
-        <v>10005</v>
-      </c>
-      <c r="W2">
+      <c r="D4">
+        <v>1411334</v>
+      </c>
+      <c r="E4">
+        <v>50007</v>
+      </c>
+      <c r="F4">
+        <v>50091</v>
+      </c>
+      <c r="G4">
+        <v>250001</v>
+      </c>
+      <c r="H4">
+        <v>250013</v>
+      </c>
+      <c r="I4">
+        <v>50016</v>
+      </c>
+      <c r="J4">
+        <v>250004</v>
+      </c>
+      <c r="K4">
+        <v>250005</v>
+      </c>
+      <c r="L4">
+        <v>250009</v>
+      </c>
+      <c r="M4">
+        <v>50018</v>
+      </c>
+      <c r="N4">
+        <v>50018</v>
+      </c>
+      <c r="O4">
+        <v>250005</v>
+      </c>
+      <c r="P4">
+        <v>50018</v>
+      </c>
+      <c r="Q4">
+        <v>250088</v>
+      </c>
+      <c r="R4">
+        <v>50019</v>
+      </c>
+      <c r="S4">
+        <v>250006</v>
+      </c>
+      <c r="T4">
         <v>50005</v>
       </c>
-      <c r="X2">
-        <v>10005</v>
-      </c>
-      <c r="Y2">
-        <v>50001</v>
-      </c>
-      <c r="Z2">
-        <v>10005</v>
-      </c>
-      <c r="AA2">
+      <c r="U4">
+        <v>250007</v>
+      </c>
+      <c r="V4">
+        <v>50007</v>
+      </c>
+      <c r="W4">
+        <v>250015</v>
+      </c>
+      <c r="X4">
+        <v>50007</v>
+      </c>
+      <c r="Y4">
+        <v>250006</v>
+      </c>
+      <c r="Z4">
         <v>50005</v>
       </c>
-      <c r="AB2">
-        <v>10011</v>
-      </c>
-      <c r="AC2">
-        <v>10545</v>
-      </c>
-      <c r="AD2">
-        <v>50071</v>
-      </c>
-      <c r="AE2">
-        <v>10932</v>
-      </c>
-      <c r="AF2">
-        <v>50001</v>
-      </c>
-      <c r="AG2">
-        <v>11322</v>
-      </c>
-      <c r="AH2">
-        <v>50010</v>
-      </c>
-      <c r="AI2">
-        <v>11941</v>
-      </c>
-      <c r="AJ2">
-        <v>249998</v>
-      </c>
-      <c r="AK2">
-        <v>12053</v>
-      </c>
-      <c r="AL2">
-        <v>250018</v>
+      <c r="AA4">
+        <v>250006</v>
+      </c>
+      <c r="AB4">
+        <v>50014</v>
+      </c>
+      <c r="AC4">
+        <v>50930</v>
+      </c>
+      <c r="AD4">
+        <v>250758</v>
+      </c>
+      <c r="AE4">
+        <v>50551</v>
+      </c>
+      <c r="AF4">
+        <v>250014</v>
+      </c>
+      <c r="AG4">
+        <v>50316</v>
+      </c>
+      <c r="AH4">
+        <v>250009</v>
+      </c>
+      <c r="AI4">
+        <v>52057</v>
+      </c>
+      <c r="AJ4">
+        <v>1774491</v>
+      </c>
+      <c r="AK4">
+        <v>51733</v>
+      </c>
+      <c r="AL4">
+        <v>1271261</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>249998</v>
-      </c>
-      <c r="C3">
-        <v>50006</v>
-      </c>
-      <c r="D3">
-        <v>1411334</v>
-      </c>
-      <c r="E3">
-        <v>50007</v>
-      </c>
-      <c r="F3">
-        <v>50091</v>
-      </c>
-      <c r="G3">
-        <v>250001</v>
-      </c>
-      <c r="H3">
-        <v>250013</v>
-      </c>
-      <c r="I3">
-        <v>50016</v>
-      </c>
-      <c r="J3">
-        <v>250004</v>
-      </c>
-      <c r="K3">
-        <v>250005</v>
-      </c>
-      <c r="L3">
-        <v>250009</v>
-      </c>
-      <c r="M3">
-        <v>50018</v>
-      </c>
-      <c r="N3">
-        <v>50018</v>
-      </c>
-      <c r="O3">
-        <v>250005</v>
-      </c>
-      <c r="P3">
-        <v>50018</v>
-      </c>
-      <c r="Q3">
-        <v>250088</v>
-      </c>
-      <c r="R3">
-        <v>50019</v>
-      </c>
-      <c r="S3">
-        <v>250006</v>
-      </c>
-      <c r="T3">
-        <v>50005</v>
-      </c>
-      <c r="U3">
-        <v>250007</v>
-      </c>
-      <c r="V3">
-        <v>50007</v>
-      </c>
-      <c r="W3">
-        <v>250015</v>
-      </c>
-      <c r="X3">
-        <v>50007</v>
-      </c>
-      <c r="Y3">
-        <v>250006</v>
-      </c>
-      <c r="Z3">
-        <v>50005</v>
-      </c>
-      <c r="AA3">
-        <v>250006</v>
-      </c>
-      <c r="AB3">
-        <v>50014</v>
-      </c>
-      <c r="AC3">
-        <v>50930</v>
-      </c>
-      <c r="AD3">
-        <v>250758</v>
-      </c>
-      <c r="AE3">
-        <v>50551</v>
-      </c>
-      <c r="AF3">
-        <v>250014</v>
-      </c>
-      <c r="AG3">
-        <v>50316</v>
-      </c>
-      <c r="AH3">
-        <v>250009</v>
-      </c>
-      <c r="AI3">
-        <v>52057</v>
-      </c>
-      <c r="AJ3">
-        <v>1774491</v>
-      </c>
-      <c r="AK3">
-        <v>51733</v>
-      </c>
-      <c r="AL3">
-        <v>1271261</v>
+    <row r="5" spans="1:38" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>166675</v>
+      </c>
+      <c r="C5">
+        <v>33339</v>
+      </c>
+      <c r="D5">
+        <v>333346</v>
+      </c>
+      <c r="E5">
+        <v>33335</v>
+      </c>
+      <c r="F5">
+        <v>33340</v>
+      </c>
+      <c r="G5">
+        <v>166673</v>
+      </c>
+      <c r="H5">
+        <v>166686</v>
+      </c>
+      <c r="I5">
+        <v>33339</v>
+      </c>
+      <c r="J5">
+        <v>166677</v>
+      </c>
+      <c r="K5">
+        <v>166673</v>
+      </c>
+      <c r="L5">
+        <v>166684</v>
+      </c>
+      <c r="M5">
+        <v>33343</v>
+      </c>
+      <c r="N5">
+        <v>33340</v>
+      </c>
+      <c r="O5">
+        <v>166673</v>
+      </c>
+      <c r="P5">
+        <v>33343</v>
+      </c>
+      <c r="Q5">
+        <v>166677</v>
+      </c>
+      <c r="R5">
+        <v>33351</v>
+      </c>
+      <c r="S5">
+        <v>166689</v>
+      </c>
+      <c r="T5">
+        <v>33350</v>
+      </c>
+      <c r="U5">
+        <v>166688</v>
+      </c>
+      <c r="V5">
+        <v>33361</v>
+      </c>
+      <c r="W5">
+        <v>166686</v>
+      </c>
+      <c r="X5">
+        <v>33352</v>
+      </c>
+      <c r="Y5">
+        <v>166678</v>
+      </c>
+      <c r="Z5">
+        <v>33337</v>
+      </c>
+      <c r="AA5">
+        <v>166684</v>
+      </c>
+      <c r="AB5">
+        <v>44665</v>
+      </c>
+      <c r="AC5">
+        <v>166745</v>
+      </c>
+      <c r="AD5">
+        <v>178029</v>
+      </c>
+      <c r="AE5">
+        <v>166679</v>
+      </c>
+      <c r="AF5">
+        <v>166682</v>
+      </c>
+      <c r="AG5">
+        <v>33812</v>
+      </c>
+      <c r="AH5">
+        <v>166678</v>
+      </c>
+      <c r="AI5">
+        <v>166692</v>
+      </c>
+      <c r="AJ5">
+        <v>333357</v>
+      </c>
+      <c r="AK5">
+        <v>166677</v>
+      </c>
+      <c r="AL5">
+        <v>333354</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>166675</v>
-      </c>
-      <c r="C4">
-        <v>33339</v>
-      </c>
-      <c r="D4">
-        <v>333346</v>
-      </c>
-      <c r="E4">
-        <v>33335</v>
-      </c>
-      <c r="F4">
-        <v>33340</v>
-      </c>
-      <c r="G4">
-        <v>166673</v>
-      </c>
-      <c r="H4">
-        <v>166686</v>
-      </c>
-      <c r="I4">
-        <v>33339</v>
-      </c>
-      <c r="J4">
-        <v>166677</v>
-      </c>
-      <c r="K4">
-        <v>166673</v>
-      </c>
-      <c r="L4">
-        <v>166684</v>
-      </c>
-      <c r="M4">
-        <v>33343</v>
-      </c>
-      <c r="N4">
-        <v>33340</v>
-      </c>
-      <c r="O4">
-        <v>166673</v>
-      </c>
-      <c r="P4">
-        <v>33343</v>
-      </c>
-      <c r="Q4">
-        <v>166677</v>
-      </c>
-      <c r="R4">
-        <v>33351</v>
-      </c>
-      <c r="S4">
-        <v>166689</v>
-      </c>
-      <c r="T4">
-        <v>33350</v>
-      </c>
-      <c r="U4">
-        <v>166688</v>
-      </c>
-      <c r="V4">
-        <v>33361</v>
-      </c>
-      <c r="W4">
-        <v>166686</v>
-      </c>
-      <c r="X4">
-        <v>33352</v>
-      </c>
-      <c r="Y4">
-        <v>166678</v>
-      </c>
-      <c r="Z4">
-        <v>33337</v>
-      </c>
-      <c r="AA4">
-        <v>166684</v>
-      </c>
-      <c r="AB4">
-        <v>44665</v>
-      </c>
-      <c r="AC4">
-        <v>166745</v>
-      </c>
-      <c r="AD4">
-        <v>178029</v>
-      </c>
-      <c r="AE4">
-        <v>166679</v>
-      </c>
-      <c r="AF4">
-        <v>166682</v>
-      </c>
-      <c r="AG4">
-        <v>33812</v>
-      </c>
-      <c r="AH4">
-        <v>166678</v>
-      </c>
-      <c r="AI4">
-        <v>166692</v>
-      </c>
-      <c r="AJ4">
-        <v>333357</v>
-      </c>
-      <c r="AK4">
-        <v>166677</v>
-      </c>
-      <c r="AL4">
-        <v>333354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:38" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>83340</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>16670</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>166672</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>16688</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>16684</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>83338</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>83343</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>16673</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <v>83337</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <v>83340</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <v>83340</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <v>16672</v>
       </c>
-      <c r="N5">
+      <c r="N6">
         <v>16675</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <v>83340</v>
       </c>
-      <c r="P5">
+      <c r="P6">
         <v>16672</v>
       </c>
-      <c r="Q5">
+      <c r="Q6">
         <v>83340</v>
       </c>
-      <c r="R5">
+      <c r="R6">
         <v>16676</v>
       </c>
-      <c r="S5">
+      <c r="S6">
         <v>83344</v>
       </c>
-      <c r="T5">
+      <c r="T6">
         <v>16674</v>
       </c>
-      <c r="U5">
+      <c r="U6">
         <v>83341</v>
       </c>
-      <c r="V5">
+      <c r="V6">
         <v>16673</v>
       </c>
-      <c r="W5">
+      <c r="W6">
         <v>83339</v>
       </c>
-      <c r="X5">
+      <c r="X6">
         <v>16681</v>
       </c>
-      <c r="Y5">
+      <c r="Y6">
         <v>83342</v>
       </c>
-      <c r="Z5">
+      <c r="Z6">
         <v>16674</v>
       </c>
-      <c r="AA5">
+      <c r="AA6">
         <v>83346</v>
       </c>
-      <c r="AB5">
+      <c r="AB6">
         <v>73674</v>
       </c>
-      <c r="AC5">
+      <c r="AC6">
         <v>83542</v>
       </c>
-      <c r="AD5">
+      <c r="AD6">
         <v>103293</v>
       </c>
-      <c r="AE5">
+      <c r="AE6">
         <v>83342</v>
       </c>
-      <c r="AF5">
+      <c r="AF6">
         <v>83349</v>
       </c>
-      <c r="AG5">
+      <c r="AG6">
         <v>83352</v>
       </c>
-      <c r="AH5">
+      <c r="AH6">
         <v>83344</v>
       </c>
-      <c r="AI5">
+      <c r="AI6">
         <v>83361</v>
       </c>
-      <c r="AJ5">
+      <c r="AJ6">
         <v>166691</v>
       </c>
-      <c r="AK5">
+      <c r="AK6">
         <v>83359</v>
       </c>
-      <c r="AL5">
+      <c r="AL6">
         <v>166684</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AL1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>